<commit_message>
petite modif sur le diagramme
</commit_message>
<xml_diff>
--- a/Others/timegap.xlsx
+++ b/Others/timegap.xlsx
@@ -594,6 +594,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Time/EpGap corrélation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
@@ -1718,17 +1737,37 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="83190336"/>
-        <c:axId val="84076224"/>
+        <c:axId val="63372608"/>
+        <c:axId val="82706432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83190336"/>
+        <c:axId val="63372608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Elapsed</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> time (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -1736,12 +1775,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84076224"/>
+        <c:crossAx val="82706432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84076224"/>
+        <c:axId val="82706432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1749,6 +1788,21 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>EpGap</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -1756,7 +1810,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83190336"/>
+        <c:crossAx val="63372608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
@@ -1776,6 +1830,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="1.3149999999999999" header="0.3" footer="0.3"/>
     <c:pageSetup paperSize="9" orientation="portrait"/>
   </c:printSettings>
+  <c:userShapes r:id="rId1"/>
 </c:chartSpace>
 </file>
 
@@ -1814,6 +1869,89 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.66901</cdr:x>
+      <cdr:y>0.05665</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.96479</cdr:x>
+      <cdr:y>0.20443</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6515100" y="350520"/>
+          <a:ext cx="2880360" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.41471</cdr:x>
+      <cdr:y>0.06404</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.94757</cdr:x>
+      <cdr:y>0.21182</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4038600" y="396240"/>
+          <a:ext cx="5189220" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Analyse sur toutes les instances qui ont une durée d'exécution &gt; 180s.</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>CPU:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t> Intel Celeron CPU B810 @ 2coeurs * 1.6GHz</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3232,7 +3370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>